<commit_message>
updated Excel Read method
</commit_message>
<xml_diff>
--- a/MyExcel.xlsx
+++ b/MyExcel.xlsx
@@ -61,7 +61,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,6 +72,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,9 +103,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,7 +411,7 @@
   <dimension ref="A2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +436,7 @@
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" t="b">
@@ -443,7 +450,7 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -472,6 +479,9 @@
       </c>
       <c r="C7" t="s">
         <v>12</v>
+      </c>
+      <c r="D7">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>